<commit_message>
Beprechungsprotokoll und kleine Änderungen im Datenbank Entwurf
19.07.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Datenbank-Entwurf/Relationenmodel.xlsx
+++ b/Datenbank-Entwurf/Relationenmodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Datenbank-Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9877523A-9C53-4BA4-9D7C-96044E317369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ABD06D-D9D6-47A9-A822-1EF0D7F82148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AC8A06F1-AA4D-4773-B2ED-BDFA6D7BEBF9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AC8A06F1-AA4D-4773-B2ED-BDFA6D7BEBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>Wartung</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Flugart</t>
   </si>
   <si>
-    <t>Flug</t>
-  </si>
-  <si>
     <t>Benutzer</t>
   </si>
   <si>
@@ -164,24 +161,9 @@
     <t>Zählerstand</t>
   </si>
   <si>
-    <t>Freigeschaltet</t>
-  </si>
-  <si>
-    <t>Typ</t>
-  </si>
-  <si>
     <t>Flugzeugtyp</t>
   </si>
   <si>
-    <t>WartungFlugzeug</t>
-  </si>
-  <si>
-    <t>FlugzeugId (Flugzeug)</t>
-  </si>
-  <si>
-    <t>WartungsId (Wartung)</t>
-  </si>
-  <si>
     <t>TypId (Typ)</t>
   </si>
   <si>
@@ -207,13 +189,25 @@
   </si>
   <si>
     <t>Flugart(Id)</t>
+  </si>
+  <si>
+    <t>Rolle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flugzeugtyp </t>
+  </si>
+  <si>
+    <t>Grounded</t>
+  </si>
+  <si>
+    <t>Start-Lande Liste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +229,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -266,33 +266,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -392,13 +375,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF44B3E1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF44B3E1"/>
         </left>
@@ -408,6 +384,31 @@
         <top style="thin">
           <color rgb="FF44B3E1"/>
         </top>
+        <bottom style="thin">
+          <color rgb="FF44B3E1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF44B3E1"/>
         </bottom>
@@ -487,12 +488,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}" name="Tabelle6" displayName="Tabelle6" ref="A21:C27" totalsRowShown="0" dataDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}" name="Tabelle6" displayName="Tabelle6" ref="A21:C27" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A21:C27" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E97089F7-F171-445E-9DE1-6793A94DDF70}" name="Attribut" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B187651B-8421-4508-B268-6C0F504846F1}" name="Datentyp" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{36FE9056-43E2-4279-9859-262819DFED19}" name="Domain" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E97089F7-F171-445E-9DE1-6793A94DDF70}" name="Attribut" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B187651B-8421-4508-B268-6C0F504846F1}" name="Datentyp" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{36FE9056-43E2-4279-9859-262819DFED19}" name="Domain" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -517,18 +518,6 @@
     <tableColumn id="1" xr3:uid="{E9B816C5-168E-47DE-8FEF-B6250BE6DF66}" name="Attribut"/>
     <tableColumn id="2" xr3:uid="{2666B0A7-F2A1-45AD-B2DB-1CEF874CD28D}" name="Datentyp"/>
     <tableColumn id="3" xr3:uid="{FD455812-D711-40DB-A6E3-526FBAF55BE8}" name="Domain"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D4C44A96-4E8B-4873-80D2-4B95DC8690B6}" name="Tabelle7910" displayName="Tabelle7910" ref="M21:O24" totalsRowShown="0">
-  <autoFilter ref="M21:O24" xr:uid="{D4C44A96-4E8B-4873-80D2-4B95DC8690B6}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{86D29508-0623-47B8-9295-602DCC9FD3CA}" name="Attribut"/>
-    <tableColumn id="2" xr3:uid="{7EB05F26-663A-4D78-9ABE-B97DDA590408}" name="Datentyp"/>
-    <tableColumn id="3" xr3:uid="{9F864E40-5296-4DBC-8608-394A6DB7CF7F}" name="Domain"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -854,7 +843,7 @@
   <dimension ref="A2:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,13 +867,13 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
-        <v>6</v>
-      </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -936,251 +925,248 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>8</v>
-      </c>
-      <c r="S4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
       <c r="M10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="I20" t="s">
-        <v>43</v>
-      </c>
-      <c r="M20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1208,127 +1194,101 @@
       <c r="K21" t="s">
         <v>3</v>
       </c>
-      <c r="M21" t="s">
-        <v>2</v>
-      </c>
-      <c r="N21" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
       <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" t="s">
-        <v>9</v>
-      </c>
       <c r="I22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" t="s">
         <v>7</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>8</v>
       </c>
-      <c r="K22" t="s">
-        <v>9</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N22" t="s">
-        <v>8</v>
-      </c>
-      <c r="O22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" t="s">
-        <v>14</v>
-      </c>
-      <c r="M23" t="s">
-        <v>46</v>
-      </c>
-      <c r="N23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F24" t="s">
-        <v>14</v>
-      </c>
-      <c r="M24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="9">
+  <tableParts count="8">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1337,7 +1297,6 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
-    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Besprechung Stand mit Julian, Fertigstellug DB-Entwürfe, Stundenaufzeichnung
24.07.2025 - Gabriel Deiac
</commit_message>
<xml_diff>
--- a/Datenbank-Entwurf/Relationenmodel.xlsx
+++ b/Datenbank-Entwurf/Relationenmodel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\DA-Digitaler_Fluplatz\Digitales-Flugplatzmanagement\Datenbank-Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ABD06D-D9D6-47A9-A822-1EF0D7F82148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7013C6-9801-4909-B3E9-2BA586AC8713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AC8A06F1-AA4D-4773-B2ED-BDFA6D7BEBF9}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
-  <si>
-    <t>Wartung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="70">
   <si>
     <t>Datentyp</t>
   </si>
@@ -65,24 +62,12 @@
     <t>NotNull</t>
   </si>
   <si>
-    <t>Wartungsdatum</t>
-  </si>
-  <si>
-    <t>NextDate</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Werkstatt</t>
-  </si>
-  <si>
     <t>varchar(255)</t>
   </si>
   <si>
-    <t>Kosten</t>
-  </si>
-  <si>
     <t>Decimal(10,2)</t>
   </si>
   <si>
@@ -92,24 +77,12 @@
     <t>Flugtyp</t>
   </si>
   <si>
-    <t>Tarif</t>
-  </si>
-  <si>
-    <t>Wartungskosten</t>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
     <t>NutNull</t>
   </si>
   <si>
-    <t>Startort</t>
-  </si>
-  <si>
-    <t>Landeort</t>
-  </si>
-  <si>
     <t>Startzeit</t>
   </si>
   <si>
@@ -179,18 +152,9 @@
     <t>Rollentyp</t>
   </si>
   <si>
-    <t>Pilot1 (Pilot)</t>
-  </si>
-  <si>
-    <t>Pilot2 (Pilot)</t>
-  </si>
-  <si>
     <t>FlugzeugId(Flugzeug)</t>
   </si>
   <si>
-    <t>Flugart(Id)</t>
-  </si>
-  <si>
     <t>Rolle</t>
   </si>
   <si>
@@ -201,6 +165,87 @@
   </si>
   <si>
     <t>Start-Lande Liste</t>
+  </si>
+  <si>
+    <t>Datum ARC</t>
+  </si>
+  <si>
+    <t>Datum Flugzeitwartung</t>
+  </si>
+  <si>
+    <t>Pilot2</t>
+  </si>
+  <si>
+    <t>Pilot1</t>
+  </si>
+  <si>
+    <t>Wartungsart</t>
+  </si>
+  <si>
+    <t>BenutzerId (Benutzer)</t>
+  </si>
+  <si>
+    <t>Preiskategorie</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Preis</t>
+  </si>
+  <si>
+    <t>PreisId (Preiskategorie)</t>
+  </si>
+  <si>
+    <t>Einflug</t>
+  </si>
+  <si>
+    <t>Ausflug</t>
+  </si>
+  <si>
+    <t>Landekosten</t>
+  </si>
+  <si>
+    <t>decimal(10,2)</t>
+  </si>
+  <si>
+    <t>Flugminutenkosten</t>
+  </si>
+  <si>
+    <t>FlugartId (Flugart)</t>
+  </si>
+  <si>
+    <t>FlugzeugId (Flugzeug)</t>
+  </si>
+  <si>
+    <t>jnt</t>
+  </si>
+  <si>
+    <t>KostenMinute</t>
+  </si>
+  <si>
+    <t>Reservierung</t>
+  </si>
+  <si>
+    <t>PilotId (Benutzer)</t>
+  </si>
+  <si>
+    <t>Gastname</t>
+  </si>
+  <si>
+    <t>Gastkontakt</t>
+  </si>
+  <si>
+    <t>Benutzerrolle</t>
+  </si>
+  <si>
+    <t>Endzeit</t>
+  </si>
+  <si>
+    <t>Pilotenflug</t>
+  </si>
+  <si>
+    <t>Datum</t>
   </si>
 </sst>
 </file>
@@ -245,7 +290,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -262,15 +307,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF44B3E1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF44B3E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,20 +485,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4C0C8C1-BB3C-421C-A80A-5BF4F04586D1}" name="Tabelle1" displayName="Tabelle1" ref="A3:C9" totalsRowShown="0">
-  <autoFilter ref="A3:C9" xr:uid="{D4C0C8C1-BB3C-421C-A80A-5BF4F04586D1}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF020715-950F-4463-9936-BC2549625B63}" name="Attribut"/>
-    <tableColumn id="2" xr3:uid="{0059CA20-BFBA-4FF6-BBD0-28A6139D9973}" name="Datentyp"/>
-    <tableColumn id="3" xr3:uid="{79ABAB21-FEE4-4CF5-A034-1C9ECDFE78CC}" name="Domain"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B4ED268-54EF-47FD-9004-21C6DA8A61D7}" name="Tabelle2" displayName="Tabelle2" ref="E3:G6" totalsRowShown="0">
-  <autoFilter ref="E3:G6" xr:uid="{1B4ED268-54EF-47FD-9004-21C6DA8A61D7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B4ED268-54EF-47FD-9004-21C6DA8A61D7}" name="Tabelle2" displayName="Tabelle2" ref="E3:G5" totalsRowShown="0">
+  <autoFilter ref="E3:G5" xr:uid="{1B4ED268-54EF-47FD-9004-21C6DA8A61D7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{68F82B24-2278-42AE-A635-F074F8640B16}" name="Attribut"/>
     <tableColumn id="2" xr3:uid="{DE151967-C5F2-417D-BB43-3C7986B455E8}" name="Datentyp"/>
@@ -451,7 +496,43 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5022BA04-5AE7-44C1-AB24-A8814A489E38}" name="Tabelle211" displayName="Tabelle211" ref="I29:K33" totalsRowShown="0">
+  <autoFilter ref="I29:K33" xr:uid="{5022BA04-5AE7-44C1-AB24-A8814A489E38}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DDC0C2A6-1127-405B-863C-2DC234C5266A}" name="Attribut"/>
+    <tableColumn id="2" xr3:uid="{A2F8300D-6E2A-4096-B9B0-D08512CE22B4}" name="Datentyp"/>
+    <tableColumn id="3" xr3:uid="{594007D6-EBE9-4FD1-97A1-4E1A69CF67E6}" name="Domain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{53B91FAE-18C3-4E26-9B4B-AA283A5DEFD9}" name="Tabelle79212" displayName="Tabelle79212" ref="A29:C38" totalsRowShown="0">
+  <autoFilter ref="A29:C38" xr:uid="{53B91FAE-18C3-4E26-9B4B-AA283A5DEFD9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4CD69DDC-1A63-4AE1-93EE-65317B7E1481}" name="Attribut"/>
+    <tableColumn id="2" xr3:uid="{0B0712FC-918B-462B-A3C6-3FEA2A5728D4}" name="Datentyp"/>
+    <tableColumn id="3" xr3:uid="{FF3A85A4-5BBC-4B11-9CC5-3D1F7D8EAD88}" name="Domain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B68F8028-C762-40D2-9E76-30C0656DD318}" name="Tabelle7921214" displayName="Tabelle7921214" ref="E29:G36" totalsRowShown="0">
+  <autoFilter ref="E29:G36" xr:uid="{B68F8028-C762-40D2-9E76-30C0656DD318}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1D9E72D9-0B2C-4EE6-A83D-3FC04CDE4063}" name="Attribut"/>
+    <tableColumn id="2" xr3:uid="{5192EF54-A8B9-46C1-9685-83FA6F257758}" name="Datentyp"/>
+    <tableColumn id="3" xr3:uid="{4A735ADF-1536-4D62-AAF8-61CA214B0358}" name="Domain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0C33B07-B6E8-4F90-A16F-36B179C3ACF8}" name="Tabelle3" displayName="Tabelle3" ref="I3:K14" totalsRowShown="0">
   <autoFilter ref="I3:K14" xr:uid="{C0C33B07-B6E8-4F90-A16F-36B179C3ACF8}"/>
   <tableColumns count="3">
@@ -463,9 +544,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70F693DD-B8D9-44EA-AFE6-6085B35B4F37}" name="Tabelle4" displayName="Tabelle4" ref="M3:O10" totalsRowShown="0">
-  <autoFilter ref="M3:O10" xr:uid="{70F693DD-B8D9-44EA-AFE6-6085B35B4F37}"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70F693DD-B8D9-44EA-AFE6-6085B35B4F37}" name="Tabelle4" displayName="Tabelle4" ref="M3:O9" totalsRowShown="0">
+  <autoFilter ref="M3:O9" xr:uid="{70F693DD-B8D9-44EA-AFE6-6085B35B4F37}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F5F8D2CE-7A87-44C0-985D-DBD7DD5DDFFE}" name="Attribut"/>
     <tableColumn id="2" xr3:uid="{1C5FF51C-44E2-42E6-81C4-46694A3620E1}" name="Datentyp"/>
@@ -475,9 +556,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{56BDF3C4-1937-4B01-A13F-A3EA10546D2C}" name="Tabelle16" displayName="Tabelle16" ref="Q3:S8" totalsRowShown="0">
-  <autoFilter ref="Q3:S8" xr:uid="{56BDF3C4-1937-4B01-A13F-A3EA10546D2C}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{56BDF3C4-1937-4B01-A13F-A3EA10546D2C}" name="Tabelle16" displayName="Tabelle16" ref="M21:O26" totalsRowShown="0">
+  <autoFilter ref="M21:O26" xr:uid="{56BDF3C4-1937-4B01-A13F-A3EA10546D2C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FC59F6DA-A7C7-4E6E-8DEC-0705C442C33F}" name="Attribut"/>
     <tableColumn id="2" xr3:uid="{45EAD6C4-A3ED-499C-A24A-BEE58EB80BDB}" name="Datentyp"/>
@@ -487,9 +568,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}" name="Tabelle6" displayName="Tabelle6" ref="A21:C27" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A21:C27" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}" name="Tabelle6" displayName="Tabelle6" ref="A3:C13" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A3:C13" xr:uid="{ADAEAC00-8963-44D3-9979-D670CBA50F22}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E97089F7-F171-445E-9DE1-6793A94DDF70}" name="Attribut" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{B187651B-8421-4508-B268-6C0F504846F1}" name="Datentyp" dataDxfId="1"/>
@@ -499,7 +580,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4FD9726D-22B2-4011-B29D-82FD9CA92F99}" name="Tabelle7" displayName="Tabelle7" ref="E21:G24" totalsRowShown="0">
   <autoFilter ref="E21:G24" xr:uid="{4FD9726D-22B2-4011-B29D-82FD9CA92F99}"/>
   <tableColumns count="3">
@@ -511,13 +592,37 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6E40A75D-0A92-4FCA-8BEB-4BB506E0C0BF}" name="Tabelle79" displayName="Tabelle79" ref="I21:K23" totalsRowShown="0">
-  <autoFilter ref="I21:K23" xr:uid="{6E40A75D-0A92-4FCA-8BEB-4BB506E0C0BF}"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6E40A75D-0A92-4FCA-8BEB-4BB506E0C0BF}" name="Tabelle79" displayName="Tabelle79" ref="E10:G12" totalsRowShown="0">
+  <autoFilter ref="E10:G12" xr:uid="{6E40A75D-0A92-4FCA-8BEB-4BB506E0C0BF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E9B816C5-168E-47DE-8FEF-B6250BE6DF66}" name="Attribut"/>
     <tableColumn id="2" xr3:uid="{2666B0A7-F2A1-45AD-B2DB-1CEF874CD28D}" name="Datentyp"/>
     <tableColumn id="3" xr3:uid="{FD455812-D711-40DB-A6E3-526FBAF55BE8}" name="Domain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB9F59B2-4D67-4E21-B867-9324F9E84C9C}" name="Tabelle792" displayName="Tabelle792" ref="A21:C24" totalsRowShown="0">
+  <autoFilter ref="A21:C24" xr:uid="{AB9F59B2-4D67-4E21-B867-9324F9E84C9C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{653C0BDD-EC0C-40A1-8215-5C10CBBFC63F}" name="Attribut"/>
+    <tableColumn id="2" xr3:uid="{1B135E49-CD33-4A58-8DCD-4C1F38029835}" name="Datentyp"/>
+    <tableColumn id="3" xr3:uid="{AA55C182-53BE-4045-9F75-3463ED0BD09F}" name="Domain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E0D30293-F989-4AF8-8931-498379AB141A}" name="Tabelle7910" displayName="Tabelle7910" ref="I21:K24" totalsRowShown="0">
+  <autoFilter ref="I21:K24" xr:uid="{E0D30293-F989-4AF8-8931-498379AB141A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0F03A5FF-A202-4039-8858-6F886CBFB340}" name="Attribut"/>
+    <tableColumn id="2" xr3:uid="{05DB2872-10F2-41EF-AD76-0BF7D0D18D63}" name="Datentyp"/>
+    <tableColumn id="3" xr3:uid="{A0425064-D59A-4CAF-AE78-389460184033}" name="Domain"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -840,455 +945,710 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EABA76-622B-4920-8F7A-A9573969787F}">
-  <dimension ref="A2:S27"/>
+  <dimension ref="A2:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.7109375" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I21" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>2</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M21" t="s">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" t="s">
+        <v>6</v>
+      </c>
+      <c r="O22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="E29" t="s">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>61</v>
+      </c>
+      <c r="J33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
         <v>35</v>
       </c>
-      <c r="R7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
-      </c>
-      <c r="J23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>44</v>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="8">
+  <tableParts count="12">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1297,6 +1657,10 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>